<commit_message>
Changed control using IA-11 to AC-6(10)
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-red-hat-enterprise-linux-6-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-red-hat-enterprise-linux-6-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-high-red-hat-enterprise-linux-6-stig-overlay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\CMS_InSpec_Profile_to_NISTSecurityControl_Maps_06132019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2860C43A-DA1E-D04E-8DC8-D59CC0A477D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D92EAA14-5F34-4BAF-969A-86AFAE6FC28B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="-552" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-rhel6-stig" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3459" uniqueCount="1994">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3460" uniqueCount="1995">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -7670,12 +7670,6 @@
 # visudo -f [other sudo configuration file]</t>
   </si>
   <si>
-    <t xml:space="preserve">CCI-002038
-The organization requires users to reauthenticate when organization-defined circumstances or situations requiring reauthentication.
-NIST SP 800-53 Revision 4 :: IA-11
-</t>
-  </si>
-  <si>
     <t>V-72817</t>
   </si>
   <si>
@@ -10850,12 +10844,44 @@
 Add to Overlay:
 desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since this requirement is not part of the ARS implementation standards.'</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-002038
+The organization requires users to reauthenticate when organization-defined circumstances or situations requiring reauthentication.
+NIST SP 800-53 Revision 4 :: IA-11
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+AC-6(10)
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">CMS ARS 3.1 does not use IA-11, however traditionally this type of finding is associated with AC-6, Least Privilege. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -11045,6 +11071,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -11412,7 +11446,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -11456,6 +11490,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -11815,26 +11852,26 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y265"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B237" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="Y1" sqref="Y1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC139" sqref="AC139"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.84765625" style="1"/>
     <col min="3" max="5" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="32.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="37.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.84765625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="37.34765625" style="2" customWidth="1"/>
     <col min="8" max="8" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="44" style="2" customWidth="1"/>
-    <col min="10" max="10" width="35.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="35.6484375" style="2" customWidth="1"/>
     <col min="11" max="22" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="14.5" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="22.33203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="22.34765625" style="1" customWidth="1"/>
     <col min="25" max="25" width="23.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11915,7 +11952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="356">
+    <row r="2" spans="1:25" ht="312">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -12029,7 +12066,7 @@
       </c>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" spans="1:25" ht="255">
+    <row r="4" spans="1:25" ht="218.4">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
@@ -12086,7 +12123,7 @@
       </c>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" spans="1:25" ht="187">
+    <row r="5" spans="1:25" ht="171.6">
       <c r="A5" s="5" t="s">
         <v>57</v>
       </c>
@@ -12143,7 +12180,7 @@
       </c>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:25" ht="187">
+    <row r="6" spans="1:25" ht="171.6">
       <c r="A6" s="5" t="s">
         <v>64</v>
       </c>
@@ -12200,7 +12237,7 @@
       </c>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" spans="1:25" ht="204">
+    <row r="7" spans="1:25" ht="156">
       <c r="A7" s="5" t="s">
         <v>73</v>
       </c>
@@ -12257,7 +12294,7 @@
       </c>
       <c r="Y7" s="4"/>
     </row>
-    <row r="8" spans="1:25" ht="204">
+    <row r="8" spans="1:25" ht="187.2">
       <c r="A8" s="5" t="s">
         <v>82</v>
       </c>
@@ -12314,7 +12351,7 @@
       </c>
       <c r="Y8" s="4"/>
     </row>
-    <row r="9" spans="1:25" ht="356">
+    <row r="9" spans="1:25" ht="312">
       <c r="A9" s="5" t="s">
         <v>89</v>
       </c>
@@ -12371,7 +12408,7 @@
       </c>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" spans="1:25" ht="187">
+    <row r="10" spans="1:25" ht="171.6">
       <c r="A10" s="5" t="s">
         <v>97</v>
       </c>
@@ -12428,7 +12465,7 @@
       </c>
       <c r="Y10" s="4"/>
     </row>
-    <row r="11" spans="1:25" ht="187">
+    <row r="11" spans="1:25" ht="171.6">
       <c r="A11" s="5" t="s">
         <v>103</v>
       </c>
@@ -12485,7 +12522,7 @@
       </c>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" spans="1:25" ht="187">
+    <row r="12" spans="1:25" ht="171.6">
       <c r="A12" s="5" t="s">
         <v>110</v>
       </c>
@@ -12542,7 +12579,7 @@
       </c>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" spans="1:25" ht="187">
+    <row r="13" spans="1:25" ht="171.6">
       <c r="A13" s="5" t="s">
         <v>117</v>
       </c>
@@ -12599,7 +12636,7 @@
       </c>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" spans="1:25" ht="340">
+    <row r="14" spans="1:25" ht="296.39999999999998">
       <c r="A14" s="5" t="s">
         <v>123</v>
       </c>
@@ -12652,11 +12689,11 @@
         <v>2367</v>
       </c>
       <c r="X14" s="6" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="Y14"/>
     </row>
-    <row r="15" spans="1:25" ht="238">
+    <row r="15" spans="1:25" ht="218.4">
       <c r="A15" s="5" t="s">
         <v>130</v>
       </c>
@@ -12713,7 +12750,7 @@
       </c>
       <c r="Y15"/>
     </row>
-    <row r="16" spans="1:25" ht="238">
+    <row r="16" spans="1:25" ht="218.4">
       <c r="A16" s="5" t="s">
         <v>137</v>
       </c>
@@ -12770,7 +12807,7 @@
       </c>
       <c r="Y16"/>
     </row>
-    <row r="17" spans="1:25" ht="187">
+    <row r="17" spans="1:25" ht="171.6">
       <c r="A17" s="5" t="s">
         <v>144</v>
       </c>
@@ -12827,7 +12864,7 @@
       </c>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" spans="1:25" ht="187">
+    <row r="18" spans="1:25" ht="171.6">
       <c r="A18" s="5" t="s">
         <v>151</v>
       </c>
@@ -12884,7 +12921,7 @@
       </c>
       <c r="Y18" s="4"/>
     </row>
-    <row r="19" spans="1:25" ht="187">
+    <row r="19" spans="1:25" ht="171.6">
       <c r="A19" s="5" t="s">
         <v>158</v>
       </c>
@@ -12941,7 +12978,7 @@
       </c>
       <c r="Y19" s="4"/>
     </row>
-    <row r="20" spans="1:25" ht="187">
+    <row r="20" spans="1:25" ht="171.6">
       <c r="A20" s="5" t="s">
         <v>165</v>
       </c>
@@ -12998,7 +13035,7 @@
       </c>
       <c r="Y20" s="4"/>
     </row>
-    <row r="21" spans="1:25" ht="187">
+    <row r="21" spans="1:25" ht="171.6">
       <c r="A21" s="5" t="s">
         <v>172</v>
       </c>
@@ -13055,7 +13092,7 @@
       </c>
       <c r="Y21" s="4"/>
     </row>
-    <row r="22" spans="1:25" ht="272">
+    <row r="22" spans="1:25" ht="234">
       <c r="A22" s="5" t="s">
         <v>178</v>
       </c>
@@ -13112,7 +13149,7 @@
       </c>
       <c r="Y22" s="4"/>
     </row>
-    <row r="23" spans="1:25" ht="187">
+    <row r="23" spans="1:25" ht="171.6">
       <c r="A23" s="5" t="s">
         <v>187</v>
       </c>
@@ -13169,7 +13206,7 @@
       </c>
       <c r="Y23" s="4"/>
     </row>
-    <row r="24" spans="1:25" ht="187">
+    <row r="24" spans="1:25" ht="171.6">
       <c r="A24" s="5" t="s">
         <v>193</v>
       </c>
@@ -13226,7 +13263,7 @@
       </c>
       <c r="Y24" s="4"/>
     </row>
-    <row r="25" spans="1:25" ht="340">
+    <row r="25" spans="1:25" ht="312">
       <c r="A25" s="5" t="s">
         <v>200</v>
       </c>
@@ -13283,7 +13320,7 @@
       </c>
       <c r="Y25"/>
     </row>
-    <row r="26" spans="1:25" ht="404">
+    <row r="26" spans="1:25" ht="358.8">
       <c r="A26" s="5" t="s">
         <v>209</v>
       </c>
@@ -13340,7 +13377,7 @@
       </c>
       <c r="Y26" s="4"/>
     </row>
-    <row r="27" spans="1:25" ht="409.6">
+    <row r="27" spans="1:25" ht="409.5">
       <c r="A27" s="5" t="s">
         <v>218</v>
       </c>
@@ -13397,7 +13434,7 @@
       </c>
       <c r="Y27" s="4"/>
     </row>
-    <row r="28" spans="1:25" ht="153">
+    <row r="28" spans="1:25" ht="140.4">
       <c r="A28" s="5" t="s">
         <v>225</v>
       </c>
@@ -13454,7 +13491,7 @@
       </c>
       <c r="Y28" s="4"/>
     </row>
-    <row r="29" spans="1:25" ht="388">
+    <row r="29" spans="1:25" ht="358.8">
       <c r="A29" s="5" t="s">
         <v>234</v>
       </c>
@@ -13507,11 +13544,11 @@
         <v>2367</v>
       </c>
       <c r="X29" s="6" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="Y29"/>
     </row>
-    <row r="30" spans="1:25" ht="340">
+    <row r="30" spans="1:25" ht="312">
       <c r="A30" s="5" t="s">
         <v>241</v>
       </c>
@@ -13568,7 +13605,7 @@
       </c>
       <c r="Y30" s="4"/>
     </row>
-    <row r="31" spans="1:25" ht="409.6">
+    <row r="31" spans="1:25" ht="409.5">
       <c r="A31" s="5" t="s">
         <v>248</v>
       </c>
@@ -13625,7 +13662,7 @@
       </c>
       <c r="Y31" s="4"/>
     </row>
-    <row r="32" spans="1:25" ht="238">
+    <row r="32" spans="1:25" ht="187.2">
       <c r="A32" s="5" t="s">
         <v>257</v>
       </c>
@@ -13682,7 +13719,7 @@
       </c>
       <c r="Y32" s="4"/>
     </row>
-    <row r="33" spans="1:25" ht="356">
+    <row r="33" spans="1:25" ht="327.60000000000002">
       <c r="A33" s="5" t="s">
         <v>266</v>
       </c>
@@ -13739,7 +13776,7 @@
       </c>
       <c r="Y33" s="4"/>
     </row>
-    <row r="34" spans="1:25" ht="187">
+    <row r="34" spans="1:25" ht="171.6">
       <c r="A34" s="5" t="s">
         <v>273</v>
       </c>
@@ -13796,7 +13833,7 @@
       </c>
       <c r="Y34" s="4"/>
     </row>
-    <row r="35" spans="1:25" ht="289">
+    <row r="35" spans="1:25" ht="265.2">
       <c r="A35" s="5" t="s">
         <v>280</v>
       </c>
@@ -13853,7 +13890,7 @@
       </c>
       <c r="Y35" s="4"/>
     </row>
-    <row r="36" spans="1:25" ht="306">
+    <row r="36" spans="1:25" ht="265.2">
       <c r="A36" s="5" t="s">
         <v>289</v>
       </c>
@@ -13910,7 +13947,7 @@
       </c>
       <c r="Y36" s="4"/>
     </row>
-    <row r="37" spans="1:25" ht="356">
+    <row r="37" spans="1:25" ht="327.60000000000002">
       <c r="A37" s="5" t="s">
         <v>298</v>
       </c>
@@ -13967,7 +14004,7 @@
       </c>
       <c r="Y37" s="4"/>
     </row>
-    <row r="38" spans="1:25" ht="221">
+    <row r="38" spans="1:25" ht="202.8">
       <c r="A38" s="8" t="s">
         <v>308</v>
       </c>
@@ -13991,10 +14028,10 @@
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="7" t="s">
+        <v>1931</v>
+      </c>
+      <c r="J38" s="7" t="s">
         <v>1932</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>1933</v>
       </c>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -14024,7 +14061,7 @@
       </c>
       <c r="Y38" s="4"/>
     </row>
-    <row r="39" spans="1:25" ht="409.6">
+    <row r="39" spans="1:25" ht="409.5">
       <c r="A39" s="5" t="s">
         <v>315</v>
       </c>
@@ -14081,7 +14118,7 @@
       </c>
       <c r="Y39" s="4"/>
     </row>
-    <row r="40" spans="1:25" ht="221">
+    <row r="40" spans="1:25" ht="202.8">
       <c r="A40" s="8" t="s">
         <v>324</v>
       </c>
@@ -14105,10 +14142,10 @@
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="7" t="s">
+        <v>1933</v>
+      </c>
+      <c r="J40" s="7" t="s">
         <v>1934</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>1935</v>
       </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -14138,7 +14175,7 @@
       </c>
       <c r="Y40" s="4"/>
     </row>
-    <row r="41" spans="1:25" ht="187">
+    <row r="41" spans="1:25" ht="171.6">
       <c r="A41" s="8" t="s">
         <v>331</v>
       </c>
@@ -14162,10 +14199,10 @@
       </c>
       <c r="H41" s="3"/>
       <c r="I41" s="7" t="s">
+        <v>1935</v>
+      </c>
+      <c r="J41" s="7" t="s">
         <v>1936</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>1937</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
@@ -14195,7 +14232,7 @@
       </c>
       <c r="Y41" s="4"/>
     </row>
-    <row r="42" spans="1:25" ht="323">
+    <row r="42" spans="1:25" ht="296.39999999999998">
       <c r="A42" s="5" t="s">
         <v>336</v>
       </c>
@@ -14252,7 +14289,7 @@
       </c>
       <c r="Y42" s="4"/>
     </row>
-    <row r="43" spans="1:25" ht="238">
+    <row r="43" spans="1:25" ht="218.4">
       <c r="A43" s="8" t="s">
         <v>345</v>
       </c>
@@ -14269,17 +14306,17 @@
         <v>348</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>349</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="7" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -14309,7 +14346,7 @@
       </c>
       <c r="Y43" s="4"/>
     </row>
-    <row r="44" spans="1:25" ht="255">
+    <row r="44" spans="1:25" ht="218.4">
       <c r="A44" s="5" t="s">
         <v>351</v>
       </c>
@@ -14366,7 +14403,7 @@
       </c>
       <c r="Y44" s="4"/>
     </row>
-    <row r="45" spans="1:25" ht="238">
+    <row r="45" spans="1:25" ht="202.8">
       <c r="A45" s="5" t="s">
         <v>360</v>
       </c>
@@ -14423,7 +14460,7 @@
       </c>
       <c r="Y45" s="4"/>
     </row>
-    <row r="46" spans="1:25" ht="323">
+    <row r="46" spans="1:25" ht="265.2">
       <c r="A46" s="5" t="s">
         <v>369</v>
       </c>
@@ -14480,7 +14517,7 @@
       </c>
       <c r="Y46" s="4"/>
     </row>
-    <row r="47" spans="1:25" ht="255">
+    <row r="47" spans="1:25" ht="218.4">
       <c r="A47" s="5" t="s">
         <v>378</v>
       </c>
@@ -14537,7 +14574,7 @@
       </c>
       <c r="Y47" s="4"/>
     </row>
-    <row r="48" spans="1:25" ht="323">
+    <row r="48" spans="1:25" ht="265.2">
       <c r="A48" s="5" t="s">
         <v>385</v>
       </c>
@@ -14594,7 +14631,7 @@
       </c>
       <c r="Y48" s="4"/>
     </row>
-    <row r="49" spans="1:25" ht="323">
+    <row r="49" spans="1:25" ht="249.6">
       <c r="A49" s="5" t="s">
         <v>394</v>
       </c>
@@ -14651,7 +14688,7 @@
       </c>
       <c r="Y49" s="4"/>
     </row>
-    <row r="50" spans="1:25" ht="289">
+    <row r="50" spans="1:25" ht="265.2">
       <c r="A50" s="5" t="s">
         <v>403</v>
       </c>
@@ -14708,7 +14745,7 @@
       </c>
       <c r="Y50" s="4"/>
     </row>
-    <row r="51" spans="1:25" ht="289">
+    <row r="51" spans="1:25" ht="265.2">
       <c r="A51" s="5" t="s">
         <v>412</v>
       </c>
@@ -14765,12 +14802,12 @@
       </c>
       <c r="Y51" s="4"/>
     </row>
-    <row r="52" spans="1:25" ht="272">
+    <row r="52" spans="1:25" ht="249.6">
       <c r="A52" s="8" t="s">
         <v>421</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>422</v>
@@ -14821,10 +14858,10 @@
         <v>429</v>
       </c>
       <c r="Y52" s="9" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="204">
+    <row r="53" spans="1:25" ht="171.6">
       <c r="A53" s="5" t="s">
         <v>430</v>
       </c>
@@ -14881,12 +14918,12 @@
       </c>
       <c r="Y53" s="4"/>
     </row>
-    <row r="54" spans="1:25" ht="272">
+    <row r="54" spans="1:25" ht="249.6">
       <c r="A54" s="8" t="s">
         <v>439</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>422</v>
@@ -14937,10 +14974,10 @@
         <v>429</v>
       </c>
       <c r="Y54" s="9" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="204">
+    <row r="55" spans="1:25" ht="156">
       <c r="A55" s="5" t="s">
         <v>446</v>
       </c>
@@ -14997,7 +15034,7 @@
       </c>
       <c r="Y55" s="4"/>
     </row>
-    <row r="56" spans="1:25" ht="221">
+    <row r="56" spans="1:25" ht="187.2">
       <c r="A56" s="5" t="s">
         <v>452</v>
       </c>
@@ -15054,7 +15091,7 @@
       </c>
       <c r="Y56" s="4"/>
     </row>
-    <row r="57" spans="1:25" ht="187">
+    <row r="57" spans="1:25" ht="171.6">
       <c r="A57" s="5" t="s">
         <v>459</v>
       </c>
@@ -15111,7 +15148,7 @@
       </c>
       <c r="Y57" s="4"/>
     </row>
-    <row r="58" spans="1:25" ht="221">
+    <row r="58" spans="1:25" ht="171.6">
       <c r="A58" s="5" t="s">
         <v>466</v>
       </c>
@@ -15168,7 +15205,7 @@
       </c>
       <c r="Y58" s="4"/>
     </row>
-    <row r="59" spans="1:25" ht="187">
+    <row r="59" spans="1:25" ht="171.6">
       <c r="A59" s="5" t="s">
         <v>475</v>
       </c>
@@ -15225,7 +15262,7 @@
       </c>
       <c r="Y59" s="4"/>
     </row>
-    <row r="60" spans="1:25" ht="187">
+    <row r="60" spans="1:25" ht="171.6">
       <c r="A60" s="5" t="s">
         <v>482</v>
       </c>
@@ -15282,7 +15319,7 @@
       </c>
       <c r="Y60" s="4"/>
     </row>
-    <row r="61" spans="1:25" ht="409.6">
+    <row r="61" spans="1:25" ht="409.5">
       <c r="A61" s="8" t="s">
         <v>489</v>
       </c>
@@ -15299,17 +15336,17 @@
         <v>492</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>493</v>
       </c>
       <c r="H61" s="3"/>
       <c r="I61" s="7" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="J61" s="7" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
@@ -15339,7 +15376,7 @@
       </c>
       <c r="Y61" s="4"/>
     </row>
-    <row r="62" spans="1:25" ht="187">
+    <row r="62" spans="1:25" ht="171.6">
       <c r="A62" s="5" t="s">
         <v>495</v>
       </c>
@@ -15396,7 +15433,7 @@
       </c>
       <c r="Y62" s="4"/>
     </row>
-    <row r="63" spans="1:25" ht="187">
+    <row r="63" spans="1:25" ht="171.6">
       <c r="A63" s="5" t="s">
         <v>502</v>
       </c>
@@ -15453,7 +15490,7 @@
       </c>
       <c r="Y63" s="4"/>
     </row>
-    <row r="64" spans="1:25" ht="187">
+    <row r="64" spans="1:25" ht="171.6">
       <c r="A64" s="5" t="s">
         <v>509</v>
       </c>
@@ -15510,7 +15547,7 @@
       </c>
       <c r="Y64" s="4"/>
     </row>
-    <row r="65" spans="1:25" ht="289">
+    <row r="65" spans="1:25" ht="265.2">
       <c r="A65" s="5" t="s">
         <v>515</v>
       </c>
@@ -15567,7 +15604,7 @@
       </c>
       <c r="Y65" s="4"/>
     </row>
-    <row r="66" spans="1:25" ht="272">
+    <row r="66" spans="1:25" ht="234">
       <c r="A66" s="5" t="s">
         <v>522</v>
       </c>
@@ -15624,7 +15661,7 @@
       </c>
       <c r="Y66" s="4"/>
     </row>
-    <row r="67" spans="1:25" ht="187">
+    <row r="67" spans="1:25" ht="156">
       <c r="A67" s="5" t="s">
         <v>531</v>
       </c>
@@ -15681,7 +15718,7 @@
       </c>
       <c r="Y67" s="4"/>
     </row>
-    <row r="68" spans="1:25" ht="272">
+    <row r="68" spans="1:25" ht="249.6">
       <c r="A68" s="5" t="s">
         <v>538</v>
       </c>
@@ -15738,7 +15775,7 @@
       </c>
       <c r="Y68" s="4"/>
     </row>
-    <row r="69" spans="1:25" ht="272">
+    <row r="69" spans="1:25" ht="249.6">
       <c r="A69" s="5" t="s">
         <v>545</v>
       </c>
@@ -15795,7 +15832,7 @@
       </c>
       <c r="Y69" s="4"/>
     </row>
-    <row r="70" spans="1:25" ht="272">
+    <row r="70" spans="1:25" ht="249.6">
       <c r="A70" s="5" t="s">
         <v>552</v>
       </c>
@@ -15852,7 +15889,7 @@
       </c>
       <c r="Y70" s="4"/>
     </row>
-    <row r="71" spans="1:25" ht="272">
+    <row r="71" spans="1:25" ht="249.6">
       <c r="A71" s="5" t="s">
         <v>559</v>
       </c>
@@ -15909,7 +15946,7 @@
       </c>
       <c r="Y71" s="4"/>
     </row>
-    <row r="72" spans="1:25" ht="255">
+    <row r="72" spans="1:25" ht="234">
       <c r="A72" s="5" t="s">
         <v>566</v>
       </c>
@@ -15966,7 +16003,7 @@
       </c>
       <c r="Y72" s="4"/>
     </row>
-    <row r="73" spans="1:25" ht="272">
+    <row r="73" spans="1:25" ht="249.6">
       <c r="A73" s="5" t="s">
         <v>575</v>
       </c>
@@ -16023,7 +16060,7 @@
       </c>
       <c r="Y73" s="4"/>
     </row>
-    <row r="74" spans="1:25" ht="409.6">
+    <row r="74" spans="1:25" ht="409.5">
       <c r="A74" s="5" t="s">
         <v>581</v>
       </c>
@@ -16080,7 +16117,7 @@
       </c>
       <c r="Y74" s="4"/>
     </row>
-    <row r="75" spans="1:25" ht="409.6">
+    <row r="75" spans="1:25" ht="409.5">
       <c r="A75" s="5" t="s">
         <v>590</v>
       </c>
@@ -16137,7 +16174,7 @@
       </c>
       <c r="Y75" s="4"/>
     </row>
-    <row r="76" spans="1:25" ht="409.6">
+    <row r="76" spans="1:25" ht="405.6">
       <c r="A76" s="5" t="s">
         <v>594</v>
       </c>
@@ -16194,7 +16231,7 @@
       </c>
       <c r="Y76" s="4"/>
     </row>
-    <row r="77" spans="1:25" ht="289">
+    <row r="77" spans="1:25" ht="265.2">
       <c r="A77" s="5" t="s">
         <v>601</v>
       </c>
@@ -16251,7 +16288,7 @@
       </c>
       <c r="Y77" s="4"/>
     </row>
-    <row r="78" spans="1:25" ht="289">
+    <row r="78" spans="1:25" ht="249.6">
       <c r="A78" s="5" t="s">
         <v>608</v>
       </c>
@@ -16308,7 +16345,7 @@
       </c>
       <c r="Y78" s="4"/>
     </row>
-    <row r="79" spans="1:25" ht="340">
+    <row r="79" spans="1:25" ht="312">
       <c r="A79" s="5" t="s">
         <v>615</v>
       </c>
@@ -16365,7 +16402,7 @@
       </c>
       <c r="Y79" s="4"/>
     </row>
-    <row r="80" spans="1:25" ht="289">
+    <row r="80" spans="1:25" ht="249.6">
       <c r="A80" s="5" t="s">
         <v>621</v>
       </c>
@@ -16422,7 +16459,7 @@
       </c>
       <c r="Y80" s="4"/>
     </row>
-    <row r="81" spans="1:25" ht="409.6">
+    <row r="81" spans="1:25" ht="405.6">
       <c r="A81" s="5" t="s">
         <v>628</v>
       </c>
@@ -16479,7 +16516,7 @@
       </c>
       <c r="Y81" s="4"/>
     </row>
-    <row r="82" spans="1:25" ht="272">
+    <row r="82" spans="1:25" ht="234">
       <c r="A82" s="5" t="s">
         <v>634</v>
       </c>
@@ -16536,7 +16573,7 @@
       </c>
       <c r="Y82" s="4"/>
     </row>
-    <row r="83" spans="1:25" ht="289">
+    <row r="83" spans="1:25" ht="265.2">
       <c r="A83" s="5" t="s">
         <v>641</v>
       </c>
@@ -16593,7 +16630,7 @@
       </c>
       <c r="Y83" s="4"/>
     </row>
-    <row r="84" spans="1:25" ht="289">
+    <row r="84" spans="1:25" ht="249.6">
       <c r="A84" s="5" t="s">
         <v>647</v>
       </c>
@@ -16650,7 +16687,7 @@
       </c>
       <c r="Y84" s="4"/>
     </row>
-    <row r="85" spans="1:25" ht="272">
+    <row r="85" spans="1:25" ht="249.6">
       <c r="A85" s="5" t="s">
         <v>653</v>
       </c>
@@ -16707,7 +16744,7 @@
       </c>
       <c r="Y85" s="4"/>
     </row>
-    <row r="86" spans="1:25" ht="289">
+    <row r="86" spans="1:25" ht="265.2">
       <c r="A86" s="5" t="s">
         <v>662</v>
       </c>
@@ -16764,7 +16801,7 @@
       </c>
       <c r="Y86" s="4"/>
     </row>
-    <row r="87" spans="1:25" ht="289">
+    <row r="87" spans="1:25" ht="265.2">
       <c r="A87" s="5" t="s">
         <v>668</v>
       </c>
@@ -16821,7 +16858,7 @@
       </c>
       <c r="Y87" s="4"/>
     </row>
-    <row r="88" spans="1:25" ht="272">
+    <row r="88" spans="1:25" ht="249.6">
       <c r="A88" s="5" t="s">
         <v>675</v>
       </c>
@@ -16878,7 +16915,7 @@
       </c>
       <c r="Y88" s="4"/>
     </row>
-    <row r="89" spans="1:25" ht="289">
+    <row r="89" spans="1:25" ht="265.2">
       <c r="A89" s="5" t="s">
         <v>682</v>
       </c>
@@ -16935,7 +16972,7 @@
       </c>
       <c r="Y89" s="4"/>
     </row>
-    <row r="90" spans="1:25" ht="272">
+    <row r="90" spans="1:25" ht="249.6">
       <c r="A90" s="5" t="s">
         <v>689</v>
       </c>
@@ -16992,7 +17029,7 @@
       </c>
       <c r="Y90" s="4"/>
     </row>
-    <row r="91" spans="1:25" ht="323">
+    <row r="91" spans="1:25" ht="296.39999999999998">
       <c r="A91" s="5" t="s">
         <v>695</v>
       </c>
@@ -17049,7 +17086,7 @@
       </c>
       <c r="Y91" s="4"/>
     </row>
-    <row r="92" spans="1:25" ht="272">
+    <row r="92" spans="1:25" ht="249.6">
       <c r="A92" s="5" t="s">
         <v>702</v>
       </c>
@@ -17106,7 +17143,7 @@
       </c>
       <c r="Y92" s="4"/>
     </row>
-    <row r="93" spans="1:25" ht="289">
+    <row r="93" spans="1:25" ht="234">
       <c r="A93" s="5" t="s">
         <v>708</v>
       </c>
@@ -17163,7 +17200,7 @@
       </c>
       <c r="Y93" s="4"/>
     </row>
-    <row r="94" spans="1:25" ht="409.6">
+    <row r="94" spans="1:25" ht="409.5">
       <c r="A94" s="5" t="s">
         <v>717</v>
       </c>
@@ -17220,7 +17257,7 @@
       </c>
       <c r="Y94" s="4"/>
     </row>
-    <row r="95" spans="1:25" ht="238">
+    <row r="95" spans="1:25" ht="202.8">
       <c r="A95" s="5" t="s">
         <v>724</v>
       </c>
@@ -17277,7 +17314,7 @@
       </c>
       <c r="Y95" s="4"/>
     </row>
-    <row r="96" spans="1:25" ht="255">
+    <row r="96" spans="1:25" ht="234">
       <c r="A96" s="5" t="s">
         <v>731</v>
       </c>
@@ -17334,7 +17371,7 @@
       </c>
       <c r="Y96" s="4"/>
     </row>
-    <row r="97" spans="1:25" ht="323">
+    <row r="97" spans="1:25" ht="296.39999999999998">
       <c r="A97" s="5" t="s">
         <v>738</v>
       </c>
@@ -17391,7 +17428,7 @@
       </c>
       <c r="Y97" s="4"/>
     </row>
-    <row r="98" spans="1:25" ht="272">
+    <row r="98" spans="1:25" ht="234">
       <c r="A98" s="5" t="s">
         <v>747</v>
       </c>
@@ -17448,7 +17485,7 @@
       </c>
       <c r="Y98" s="4"/>
     </row>
-    <row r="99" spans="1:25" ht="323">
+    <row r="99" spans="1:25" ht="296.39999999999998">
       <c r="A99" s="5" t="s">
         <v>753</v>
       </c>
@@ -17505,7 +17542,7 @@
       </c>
       <c r="Y99" s="4"/>
     </row>
-    <row r="100" spans="1:25" ht="323">
+    <row r="100" spans="1:25" ht="296.39999999999998">
       <c r="A100" s="5" t="s">
         <v>759</v>
       </c>
@@ -17562,7 +17599,7 @@
       </c>
       <c r="Y100" s="4"/>
     </row>
-    <row r="101" spans="1:25" ht="323">
+    <row r="101" spans="1:25" ht="296.39999999999998">
       <c r="A101" s="5" t="s">
         <v>765</v>
       </c>
@@ -17619,7 +17656,7 @@
       </c>
       <c r="Y101" s="4"/>
     </row>
-    <row r="102" spans="1:25" ht="289">
+    <row r="102" spans="1:25" ht="265.2">
       <c r="A102" s="5" t="s">
         <v>772</v>
       </c>
@@ -17676,7 +17713,7 @@
       </c>
       <c r="Y102" s="4"/>
     </row>
-    <row r="103" spans="1:25" ht="323">
+    <row r="103" spans="1:25" ht="296.39999999999998">
       <c r="A103" s="5" t="s">
         <v>781</v>
       </c>
@@ -17733,7 +17770,7 @@
       </c>
       <c r="Y103" s="4"/>
     </row>
-    <row r="104" spans="1:25" ht="306">
+    <row r="104" spans="1:25" ht="280.8">
       <c r="A104" s="5" t="s">
         <v>787</v>
       </c>
@@ -17790,7 +17827,7 @@
       </c>
       <c r="Y104" s="4"/>
     </row>
-    <row r="105" spans="1:25" ht="323">
+    <row r="105" spans="1:25" ht="296.39999999999998">
       <c r="A105" s="5" t="s">
         <v>794</v>
       </c>
@@ -17847,7 +17884,7 @@
       </c>
       <c r="Y105" s="4"/>
     </row>
-    <row r="106" spans="1:25" ht="289">
+    <row r="106" spans="1:25" ht="265.2">
       <c r="A106" s="5" t="s">
         <v>800</v>
       </c>
@@ -17904,7 +17941,7 @@
       </c>
       <c r="Y106" s="4"/>
     </row>
-    <row r="107" spans="1:25" ht="323">
+    <row r="107" spans="1:25" ht="296.39999999999998">
       <c r="A107" s="5" t="s">
         <v>804</v>
       </c>
@@ -17961,7 +17998,7 @@
       </c>
       <c r="Y107" s="4"/>
     </row>
-    <row r="108" spans="1:25" ht="255">
+    <row r="108" spans="1:25" ht="234">
       <c r="A108" s="5" t="s">
         <v>810</v>
       </c>
@@ -18018,7 +18055,7 @@
       </c>
       <c r="Y108" s="4"/>
     </row>
-    <row r="109" spans="1:25" ht="356">
+    <row r="109" spans="1:25" ht="296.39999999999998">
       <c r="A109" s="5" t="s">
         <v>814</v>
       </c>
@@ -18075,7 +18112,7 @@
       </c>
       <c r="Y109" s="4"/>
     </row>
-    <row r="110" spans="1:25" ht="323">
+    <row r="110" spans="1:25" ht="296.39999999999998">
       <c r="A110" s="5" t="s">
         <v>820</v>
       </c>
@@ -18132,7 +18169,7 @@
       </c>
       <c r="Y110" s="4"/>
     </row>
-    <row r="111" spans="1:25" ht="323">
+    <row r="111" spans="1:25" ht="296.39999999999998">
       <c r="A111" s="5" t="s">
         <v>826</v>
       </c>
@@ -18189,7 +18226,7 @@
       </c>
       <c r="Y111" s="4"/>
     </row>
-    <row r="112" spans="1:25" ht="356">
+    <row r="112" spans="1:25" ht="296.39999999999998">
       <c r="A112" s="5" t="s">
         <v>832</v>
       </c>
@@ -18246,7 +18283,7 @@
       </c>
       <c r="Y112" s="4"/>
     </row>
-    <row r="113" spans="1:25" ht="306">
+    <row r="113" spans="1:25" ht="280.8">
       <c r="A113" s="5" t="s">
         <v>838</v>
       </c>
@@ -18303,7 +18340,7 @@
       </c>
       <c r="Y113" s="4"/>
     </row>
-    <row r="114" spans="1:25" ht="323">
+    <row r="114" spans="1:25" ht="296.39999999999998">
       <c r="A114" s="5" t="s">
         <v>842</v>
       </c>
@@ -18360,7 +18397,7 @@
       </c>
       <c r="Y114" s="4"/>
     </row>
-    <row r="115" spans="1:25" ht="356">
+    <row r="115" spans="1:25" ht="296.39999999999998">
       <c r="A115" s="5" t="s">
         <v>848</v>
       </c>
@@ -18417,7 +18454,7 @@
       </c>
       <c r="Y115" s="4"/>
     </row>
-    <row r="116" spans="1:25" ht="323">
+    <row r="116" spans="1:25" ht="296.39999999999998">
       <c r="A116" s="5" t="s">
         <v>854</v>
       </c>
@@ -18474,7 +18511,7 @@
       </c>
       <c r="Y116" s="4"/>
     </row>
-    <row r="117" spans="1:25" ht="409.6">
+    <row r="117" spans="1:25" ht="358.8">
       <c r="A117" s="5" t="s">
         <v>860</v>
       </c>
@@ -18531,7 +18568,7 @@
       </c>
       <c r="Y117" s="4"/>
     </row>
-    <row r="118" spans="1:25" ht="356">
+    <row r="118" spans="1:25" ht="312">
       <c r="A118" s="5" t="s">
         <v>867</v>
       </c>
@@ -18588,7 +18625,7 @@
       </c>
       <c r="Y118" s="4"/>
     </row>
-    <row r="119" spans="1:25" ht="238">
+    <row r="119" spans="1:25" ht="202.8">
       <c r="A119" s="5" t="s">
         <v>876</v>
       </c>
@@ -18645,7 +18682,7 @@
       </c>
       <c r="Y119" s="4"/>
     </row>
-    <row r="120" spans="1:25" ht="272">
+    <row r="120" spans="1:25" ht="234">
       <c r="A120" s="8" t="s">
         <v>883</v>
       </c>
@@ -18662,17 +18699,17 @@
         <v>886</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="G120" s="4" t="s">
         <v>887</v>
       </c>
       <c r="H120" s="3"/>
       <c r="I120" s="7" t="s">
+        <v>1970</v>
+      </c>
+      <c r="J120" s="7" t="s">
         <v>1971</v>
-      </c>
-      <c r="J120" s="7" t="s">
-        <v>1972</v>
       </c>
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
@@ -18702,7 +18739,7 @@
       </c>
       <c r="Y120" s="4"/>
     </row>
-    <row r="121" spans="1:25" ht="255">
+    <row r="121" spans="1:25" ht="234">
       <c r="A121" s="8" t="s">
         <v>889</v>
       </c>
@@ -18719,17 +18756,17 @@
         <v>892</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="G121" s="4" t="s">
         <v>893</v>
       </c>
       <c r="H121" s="3"/>
       <c r="I121" s="7" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
@@ -18759,7 +18796,7 @@
       </c>
       <c r="Y121" s="4"/>
     </row>
-    <row r="122" spans="1:25" ht="255">
+    <row r="122" spans="1:25" ht="234">
       <c r="A122" s="8" t="s">
         <v>895</v>
       </c>
@@ -18776,17 +18813,17 @@
         <v>898</v>
       </c>
       <c r="F122" s="7" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="G122" s="4" t="s">
         <v>899</v>
       </c>
       <c r="H122" s="3"/>
       <c r="I122" s="7" t="s">
+        <v>1944</v>
+      </c>
+      <c r="J122" s="7" t="s">
         <v>1945</v>
-      </c>
-      <c r="J122" s="7" t="s">
-        <v>1946</v>
       </c>
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
@@ -18816,7 +18853,7 @@
       </c>
       <c r="Y122" s="4"/>
     </row>
-    <row r="123" spans="1:25" ht="289">
+    <row r="123" spans="1:25" ht="265.2">
       <c r="A123" s="8" t="s">
         <v>901</v>
       </c>
@@ -18833,17 +18870,17 @@
         <v>904</v>
       </c>
       <c r="F123" s="7" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="G123" s="4" t="s">
         <v>905</v>
       </c>
       <c r="H123" s="3"/>
       <c r="I123" s="7" t="s">
+        <v>1947</v>
+      </c>
+      <c r="J123" s="7" t="s">
         <v>1948</v>
-      </c>
-      <c r="J123" s="7" t="s">
-        <v>1949</v>
       </c>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
@@ -18873,7 +18910,7 @@
       </c>
       <c r="Y123" s="4"/>
     </row>
-    <row r="124" spans="1:25" ht="409.6">
+    <row r="124" spans="1:25" ht="409.5">
       <c r="A124" s="8" t="s">
         <v>907</v>
       </c>
@@ -18890,17 +18927,17 @@
         <v>910</v>
       </c>
       <c r="F124" s="7" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="G124" s="4" t="s">
         <v>911</v>
       </c>
       <c r="H124" s="3"/>
       <c r="I124" s="7" t="s">
+        <v>1950</v>
+      </c>
+      <c r="J124" s="7" t="s">
         <v>1951</v>
-      </c>
-      <c r="J124" s="7" t="s">
-        <v>1952</v>
       </c>
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
@@ -18930,7 +18967,7 @@
       </c>
       <c r="Y124" s="4"/>
     </row>
-    <row r="125" spans="1:25" ht="409.6">
+    <row r="125" spans="1:25" ht="409.5">
       <c r="A125" s="5" t="s">
         <v>913</v>
       </c>
@@ -18987,7 +19024,7 @@
       </c>
       <c r="Y125" s="4"/>
     </row>
-    <row r="126" spans="1:25" ht="409.6">
+    <row r="126" spans="1:25" ht="409.5">
       <c r="A126" s="5" t="s">
         <v>922</v>
       </c>
@@ -19044,7 +19081,7 @@
       </c>
       <c r="Y126" s="4"/>
     </row>
-    <row r="127" spans="1:25" ht="323">
+    <row r="127" spans="1:25" ht="296.39999999999998">
       <c r="A127" s="5" t="s">
         <v>929</v>
       </c>
@@ -19101,7 +19138,7 @@
       </c>
       <c r="Y127" s="4"/>
     </row>
-    <row r="128" spans="1:25" ht="323">
+    <row r="128" spans="1:25" ht="296.39999999999998">
       <c r="A128" s="5" t="s">
         <v>935</v>
       </c>
@@ -19158,7 +19195,7 @@
       </c>
       <c r="Y128" s="4"/>
     </row>
-    <row r="129" spans="1:25" ht="238">
+    <row r="129" spans="1:25" ht="202.8">
       <c r="A129" s="5" t="s">
         <v>941</v>
       </c>
@@ -19215,7 +19252,7 @@
       </c>
       <c r="Y129" s="4"/>
     </row>
-    <row r="130" spans="1:25" ht="187">
+    <row r="130" spans="1:25" ht="171.6">
       <c r="A130" s="5" t="s">
         <v>948</v>
       </c>
@@ -19272,7 +19309,7 @@
       </c>
       <c r="Y130" s="4"/>
     </row>
-    <row r="131" spans="1:25" ht="409.6">
+    <row r="131" spans="1:25" ht="409.5">
       <c r="A131" s="5" t="s">
         <v>955</v>
       </c>
@@ -19329,7 +19366,7 @@
       </c>
       <c r="Y131" s="4"/>
     </row>
-    <row r="132" spans="1:25" ht="187">
+    <row r="132" spans="1:25" ht="171.6">
       <c r="A132" s="5" t="s">
         <v>962</v>
       </c>
@@ -19386,7 +19423,7 @@
       </c>
       <c r="Y132" s="4"/>
     </row>
-    <row r="133" spans="1:25" ht="409.6">
+    <row r="133" spans="1:25" ht="409.5">
       <c r="A133" s="5" t="s">
         <v>969</v>
       </c>
@@ -19443,7 +19480,7 @@
       </c>
       <c r="Y133" s="4"/>
     </row>
-    <row r="134" spans="1:25" ht="388">
+    <row r="134" spans="1:25" ht="343.2">
       <c r="A134" s="5" t="s">
         <v>976</v>
       </c>
@@ -19500,7 +19537,7 @@
       </c>
       <c r="Y134" s="4"/>
     </row>
-    <row r="135" spans="1:25" ht="272">
+    <row r="135" spans="1:25" ht="249.6">
       <c r="A135" s="5" t="s">
         <v>983</v>
       </c>
@@ -19557,7 +19594,7 @@
       </c>
       <c r="Y135" s="4"/>
     </row>
-    <row r="136" spans="1:25" ht="289">
+    <row r="136" spans="1:25" ht="265.2">
       <c r="A136" s="5" t="s">
         <v>990</v>
       </c>
@@ -19614,7 +19651,7 @@
       </c>
       <c r="Y136" s="4"/>
     </row>
-    <row r="137" spans="1:25" ht="272">
+    <row r="137" spans="1:25" ht="234">
       <c r="A137" s="5" t="s">
         <v>999</v>
       </c>
@@ -19671,7 +19708,7 @@
       </c>
       <c r="Y137" s="4"/>
     </row>
-    <row r="138" spans="1:25" ht="221">
+    <row r="138" spans="1:25" ht="202.8">
       <c r="A138" s="5" t="s">
         <v>1006</v>
       </c>
@@ -19728,7 +19765,7 @@
       </c>
       <c r="Y138" s="4"/>
     </row>
-    <row r="139" spans="1:25" ht="272">
+    <row r="139" spans="1:25" ht="234">
       <c r="A139" s="5" t="s">
         <v>1015</v>
       </c>
@@ -19785,7 +19822,7 @@
       </c>
       <c r="Y139" s="4"/>
     </row>
-    <row r="140" spans="1:25" ht="306">
+    <row r="140" spans="1:25" ht="280.8">
       <c r="A140" s="5" t="s">
         <v>1022</v>
       </c>
@@ -19842,7 +19879,7 @@
       </c>
       <c r="Y140" s="4"/>
     </row>
-    <row r="141" spans="1:25" ht="238">
+    <row r="141" spans="1:25" ht="218.4">
       <c r="A141" s="5" t="s">
         <v>1031</v>
       </c>
@@ -19899,7 +19936,7 @@
       </c>
       <c r="Y141" s="4"/>
     </row>
-    <row r="142" spans="1:25" ht="221">
+    <row r="142" spans="1:25" ht="202.8">
       <c r="A142" s="5" t="s">
         <v>1038</v>
       </c>
@@ -19956,7 +19993,7 @@
       </c>
       <c r="Y142" s="4"/>
     </row>
-    <row r="143" spans="1:25" ht="409.6">
+    <row r="143" spans="1:25" ht="409.5">
       <c r="A143" s="8" t="s">
         <v>1045</v>
       </c>
@@ -19973,17 +20010,17 @@
         <v>1048</v>
       </c>
       <c r="F143" s="7" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="G143" s="7" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="H143" s="3"/>
       <c r="I143" s="7" t="s">
+        <v>1983</v>
+      </c>
+      <c r="J143" s="7" t="s">
         <v>1984</v>
-      </c>
-      <c r="J143" s="7" t="s">
-        <v>1985</v>
       </c>
       <c r="K143" s="3"/>
       <c r="L143" s="3"/>
@@ -20013,7 +20050,7 @@
       </c>
       <c r="Y143"/>
     </row>
-    <row r="144" spans="1:25" ht="409.6">
+    <row r="144" spans="1:25" ht="409.5">
       <c r="A144" s="8" t="s">
         <v>1050</v>
       </c>
@@ -20030,17 +20067,17 @@
         <v>1053</v>
       </c>
       <c r="F144" s="7" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="G144" s="4" t="s">
         <v>1054</v>
       </c>
       <c r="H144" s="3"/>
       <c r="I144" s="7" t="s">
+        <v>1953</v>
+      </c>
+      <c r="J144" s="7" t="s">
         <v>1954</v>
-      </c>
-      <c r="J144" s="7" t="s">
-        <v>1955</v>
       </c>
       <c r="K144" s="3"/>
       <c r="L144" s="3"/>
@@ -20070,7 +20107,7 @@
       </c>
       <c r="Y144" s="4"/>
     </row>
-    <row r="145" spans="1:25" ht="306">
+    <row r="145" spans="1:25" ht="265.2">
       <c r="A145" s="5" t="s">
         <v>1056</v>
       </c>
@@ -20127,7 +20164,7 @@
       </c>
       <c r="Y145" s="4"/>
     </row>
-    <row r="146" spans="1:25" ht="356">
+    <row r="146" spans="1:25" ht="312">
       <c r="A146" s="5" t="s">
         <v>1065</v>
       </c>
@@ -20184,7 +20221,7 @@
       </c>
       <c r="Y146" s="4"/>
     </row>
-    <row r="147" spans="1:25" ht="221">
+    <row r="147" spans="1:25" ht="202.8">
       <c r="A147" s="5" t="s">
         <v>1074</v>
       </c>
@@ -20241,7 +20278,7 @@
       </c>
       <c r="Y147" s="4"/>
     </row>
-    <row r="148" spans="1:25" ht="221">
+    <row r="148" spans="1:25" ht="202.8">
       <c r="A148" s="5" t="s">
         <v>1081</v>
       </c>
@@ -20298,7 +20335,7 @@
       </c>
       <c r="Y148" s="4"/>
     </row>
-    <row r="149" spans="1:25" ht="306">
+    <row r="149" spans="1:25" ht="280.8">
       <c r="A149" s="5" t="s">
         <v>1088</v>
       </c>
@@ -20355,7 +20392,7 @@
       </c>
       <c r="Y149" s="4"/>
     </row>
-    <row r="150" spans="1:25" ht="372">
+    <row r="150" spans="1:25" ht="327.60000000000002">
       <c r="A150" s="5" t="s">
         <v>1095</v>
       </c>
@@ -20412,7 +20449,7 @@
       </c>
       <c r="Y150" s="4"/>
     </row>
-    <row r="151" spans="1:25" ht="289">
+    <row r="151" spans="1:25" ht="265.2">
       <c r="A151" s="5" t="s">
         <v>1104</v>
       </c>
@@ -20469,7 +20506,7 @@
       </c>
       <c r="Y151" s="4"/>
     </row>
-    <row r="152" spans="1:25" ht="272">
+    <row r="152" spans="1:25" ht="249.6">
       <c r="A152" s="5" t="s">
         <v>1111</v>
       </c>
@@ -20526,7 +20563,7 @@
       </c>
       <c r="Y152" s="4"/>
     </row>
-    <row r="153" spans="1:25" ht="323">
+    <row r="153" spans="1:25" ht="296.39999999999998">
       <c r="A153" s="5" t="s">
         <v>1117</v>
       </c>
@@ -20583,7 +20620,7 @@
       </c>
       <c r="Y153" s="4"/>
     </row>
-    <row r="154" spans="1:25" ht="221">
+    <row r="154" spans="1:25" ht="202.8">
       <c r="A154" s="5" t="s">
         <v>1124</v>
       </c>
@@ -20640,7 +20677,7 @@
       </c>
       <c r="Y154" s="4"/>
     </row>
-    <row r="155" spans="1:25" ht="409.6">
+    <row r="155" spans="1:25" ht="390">
       <c r="A155" s="5" t="s">
         <v>1131</v>
       </c>
@@ -20697,7 +20734,7 @@
       </c>
       <c r="Y155" s="4"/>
     </row>
-    <row r="156" spans="1:25" ht="204">
+    <row r="156" spans="1:25" ht="187.2">
       <c r="A156" s="5" t="s">
         <v>1138</v>
       </c>
@@ -20754,7 +20791,7 @@
       </c>
       <c r="Y156" s="4"/>
     </row>
-    <row r="157" spans="1:25" ht="221">
+    <row r="157" spans="1:25" ht="202.8">
       <c r="A157" s="5" t="s">
         <v>1145</v>
       </c>
@@ -20811,7 +20848,7 @@
       </c>
       <c r="Y157" s="4"/>
     </row>
-    <row r="158" spans="1:25" ht="221">
+    <row r="158" spans="1:25" ht="202.8">
       <c r="A158" s="5" t="s">
         <v>1152</v>
       </c>
@@ -20868,7 +20905,7 @@
       </c>
       <c r="Y158" s="4"/>
     </row>
-    <row r="159" spans="1:25" ht="356">
+    <row r="159" spans="1:25" ht="312">
       <c r="A159" s="8" t="s">
         <v>1161</v>
       </c>
@@ -20892,10 +20929,10 @@
       </c>
       <c r="H159" s="3"/>
       <c r="I159" s="7" t="s">
+        <v>1955</v>
+      </c>
+      <c r="J159" s="7" t="s">
         <v>1956</v>
-      </c>
-      <c r="J159" s="7" t="s">
-        <v>1957</v>
       </c>
       <c r="K159" s="3"/>
       <c r="L159" s="3"/>
@@ -20925,7 +20962,7 @@
       </c>
       <c r="Y159" s="4"/>
     </row>
-    <row r="160" spans="1:25" ht="306">
+    <row r="160" spans="1:25" ht="265.2">
       <c r="A160" s="5" t="s">
         <v>1168</v>
       </c>
@@ -20982,7 +21019,7 @@
       </c>
       <c r="Y160" s="4"/>
     </row>
-    <row r="161" spans="1:25" ht="409.6">
+    <row r="161" spans="1:25" ht="390">
       <c r="A161" s="8" t="s">
         <v>1175</v>
       </c>
@@ -21035,11 +21072,11 @@
         <v>2367</v>
       </c>
       <c r="X161" s="7" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="Y161"/>
     </row>
-    <row r="162" spans="1:25" ht="388">
+    <row r="162" spans="1:25" ht="358.8">
       <c r="A162" s="8" t="s">
         <v>1183</v>
       </c>
@@ -21092,11 +21129,11 @@
         <v>2367</v>
       </c>
       <c r="X162" s="12" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="Y162"/>
     </row>
-    <row r="163" spans="1:25" ht="388">
+    <row r="163" spans="1:25" ht="358.8">
       <c r="A163" s="8" t="s">
         <v>1192</v>
       </c>
@@ -21149,11 +21186,11 @@
         <v>2367</v>
       </c>
       <c r="X163" s="12" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="Y163"/>
     </row>
-    <row r="164" spans="1:25" ht="272">
+    <row r="164" spans="1:25" ht="249.6">
       <c r="A164" s="5" t="s">
         <v>1198</v>
       </c>
@@ -21210,7 +21247,7 @@
       </c>
       <c r="Y164" s="4"/>
     </row>
-    <row r="165" spans="1:25" ht="221">
+    <row r="165" spans="1:25" ht="202.8">
       <c r="A165" s="5" t="s">
         <v>1205</v>
       </c>
@@ -21267,7 +21304,7 @@
       </c>
       <c r="Y165" s="4"/>
     </row>
-    <row r="166" spans="1:25" ht="372">
+    <row r="166" spans="1:25" ht="327.60000000000002">
       <c r="A166" s="8" t="s">
         <v>1212</v>
       </c>
@@ -21284,7 +21321,7 @@
         <v>1214</v>
       </c>
       <c r="F166" s="7" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="G166" s="4" t="s">
         <v>1215</v>
@@ -21324,7 +21361,7 @@
       </c>
       <c r="Y166" s="4"/>
     </row>
-    <row r="167" spans="1:25" ht="289">
+    <row r="167" spans="1:25" ht="265.2">
       <c r="A167" s="5" t="s">
         <v>1218</v>
       </c>
@@ -21381,7 +21418,7 @@
       </c>
       <c r="Y167" s="4"/>
     </row>
-    <row r="168" spans="1:25" ht="272">
+    <row r="168" spans="1:25" ht="234">
       <c r="A168" s="5" t="s">
         <v>1227</v>
       </c>
@@ -21438,7 +21475,7 @@
       </c>
       <c r="Y168" s="4"/>
     </row>
-    <row r="169" spans="1:25" ht="409.6">
+    <row r="169" spans="1:25" ht="405.6">
       <c r="A169" s="5" t="s">
         <v>1236</v>
       </c>
@@ -21495,7 +21532,7 @@
       </c>
       <c r="Y169" s="4"/>
     </row>
-    <row r="170" spans="1:25" ht="255">
+    <row r="170" spans="1:25" ht="234">
       <c r="A170" s="5" t="s">
         <v>1243</v>
       </c>
@@ -21552,7 +21589,7 @@
       </c>
       <c r="Y170" s="4"/>
     </row>
-    <row r="171" spans="1:25" ht="255">
+    <row r="171" spans="1:25" ht="202.8">
       <c r="A171" s="5" t="s">
         <v>1252</v>
       </c>
@@ -21609,7 +21646,7 @@
       </c>
       <c r="Y171" s="4"/>
     </row>
-    <row r="172" spans="1:25" ht="255">
+    <row r="172" spans="1:25" ht="218.4">
       <c r="A172" s="8" t="s">
         <v>1261</v>
       </c>
@@ -21626,7 +21663,7 @@
         <v>1263</v>
       </c>
       <c r="F172" s="7" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="G172" s="4" t="s">
         <v>1264</v>
@@ -21666,7 +21703,7 @@
       </c>
       <c r="Y172" s="4"/>
     </row>
-    <row r="173" spans="1:25" ht="272">
+    <row r="173" spans="1:25" ht="249.6">
       <c r="A173" s="5" t="s">
         <v>1267</v>
       </c>
@@ -21723,7 +21760,7 @@
       </c>
       <c r="Y173" s="4"/>
     </row>
-    <row r="174" spans="1:25" ht="306">
+    <row r="174" spans="1:25" ht="265.2">
       <c r="A174" s="5" t="s">
         <v>1274</v>
       </c>
@@ -21780,7 +21817,7 @@
       </c>
       <c r="Y174" s="4"/>
     </row>
-    <row r="175" spans="1:25" ht="187">
+    <row r="175" spans="1:25" ht="171.6">
       <c r="A175" s="5" t="s">
         <v>1281</v>
       </c>
@@ -21837,7 +21874,7 @@
       </c>
       <c r="Y175" s="4"/>
     </row>
-    <row r="176" spans="1:25" ht="204">
+    <row r="176" spans="1:25" ht="187.2">
       <c r="A176" s="5" t="s">
         <v>1288</v>
       </c>
@@ -21894,7 +21931,7 @@
       </c>
       <c r="Y176" s="4"/>
     </row>
-    <row r="177" spans="1:25" ht="255">
+    <row r="177" spans="1:25" ht="218.4">
       <c r="A177" s="5" t="s">
         <v>1295</v>
       </c>
@@ -21951,7 +21988,7 @@
       </c>
       <c r="Y177" s="4"/>
     </row>
-    <row r="178" spans="1:25" ht="221">
+    <row r="178" spans="1:25" ht="202.8">
       <c r="A178" s="5" t="s">
         <v>1304</v>
       </c>
@@ -22008,7 +22045,7 @@
       </c>
       <c r="Y178" s="4"/>
     </row>
-    <row r="179" spans="1:25" ht="238">
+    <row r="179" spans="1:25" ht="202.8">
       <c r="A179" s="5" t="s">
         <v>1313</v>
       </c>
@@ -22065,7 +22102,7 @@
       </c>
       <c r="Y179" s="4"/>
     </row>
-    <row r="180" spans="1:25" ht="204">
+    <row r="180" spans="1:25" ht="187.2">
       <c r="A180" s="5" t="s">
         <v>1320</v>
       </c>
@@ -22122,7 +22159,7 @@
       </c>
       <c r="Y180" s="4"/>
     </row>
-    <row r="181" spans="1:25" ht="221">
+    <row r="181" spans="1:25" ht="187.2">
       <c r="A181" s="5" t="s">
         <v>1326</v>
       </c>
@@ -22179,7 +22216,7 @@
       </c>
       <c r="Y181" s="4"/>
     </row>
-    <row r="182" spans="1:25" ht="221">
+    <row r="182" spans="1:25" ht="202.8">
       <c r="A182" s="5" t="s">
         <v>1332</v>
       </c>
@@ -22236,7 +22273,7 @@
       </c>
       <c r="Y182"/>
     </row>
-    <row r="183" spans="1:25" ht="388">
+    <row r="183" spans="1:25" ht="358.8">
       <c r="A183" s="5" t="s">
         <v>1339</v>
       </c>
@@ -22293,7 +22330,7 @@
       </c>
       <c r="Y183" s="4"/>
     </row>
-    <row r="184" spans="1:25" ht="187">
+    <row r="184" spans="1:25" ht="171.6">
       <c r="A184" s="5" t="s">
         <v>1346</v>
       </c>
@@ -22350,7 +22387,7 @@
       </c>
       <c r="Y184" s="4"/>
     </row>
-    <row r="185" spans="1:25" ht="356">
+    <row r="185" spans="1:25" ht="327.60000000000002">
       <c r="A185" s="5" t="s">
         <v>1352</v>
       </c>
@@ -22407,7 +22444,7 @@
       </c>
       <c r="Y185" s="4"/>
     </row>
-    <row r="186" spans="1:25" ht="221">
+    <row r="186" spans="1:25" ht="202.8">
       <c r="A186" s="5" t="s">
         <v>1361</v>
       </c>
@@ -22464,7 +22501,7 @@
       </c>
       <c r="Y186" s="4"/>
     </row>
-    <row r="187" spans="1:25" ht="255">
+    <row r="187" spans="1:25" ht="234">
       <c r="A187" s="5" t="s">
         <v>1368</v>
       </c>
@@ -22521,7 +22558,7 @@
       </c>
       <c r="Y187" s="4"/>
     </row>
-    <row r="188" spans="1:25" ht="409.6">
+    <row r="188" spans="1:25" ht="390">
       <c r="A188" s="5" t="s">
         <v>1377</v>
       </c>
@@ -22578,7 +22615,7 @@
       </c>
       <c r="Y188" s="4"/>
     </row>
-    <row r="189" spans="1:25" ht="409.6">
+    <row r="189" spans="1:25" ht="409.5">
       <c r="A189" s="5" t="s">
         <v>1384</v>
       </c>
@@ -22635,7 +22672,7 @@
       </c>
       <c r="Y189" s="4"/>
     </row>
-    <row r="190" spans="1:25" ht="289">
+    <row r="190" spans="1:25" ht="249.6">
       <c r="A190" s="5" t="s">
         <v>1391</v>
       </c>
@@ -22692,7 +22729,7 @@
       </c>
       <c r="Y190" s="4"/>
     </row>
-    <row r="191" spans="1:25" ht="187">
+    <row r="191" spans="1:25" ht="171.6">
       <c r="A191" s="5" t="s">
         <v>1398</v>
       </c>
@@ -22749,7 +22786,7 @@
       </c>
       <c r="Y191" s="4"/>
     </row>
-    <row r="192" spans="1:25" ht="409.6">
+    <row r="192" spans="1:25" ht="390">
       <c r="A192" s="5" t="s">
         <v>1405</v>
       </c>
@@ -22806,7 +22843,7 @@
       </c>
       <c r="Y192" s="4"/>
     </row>
-    <row r="193" spans="1:25" ht="255">
+    <row r="193" spans="1:25" ht="234">
       <c r="A193" s="5" t="s">
         <v>1412</v>
       </c>
@@ -22863,7 +22900,7 @@
       </c>
       <c r="Y193" s="4"/>
     </row>
-    <row r="194" spans="1:25" ht="409.6">
+    <row r="194" spans="1:25" ht="390">
       <c r="A194" s="5" t="s">
         <v>1419</v>
       </c>
@@ -22920,7 +22957,7 @@
       </c>
       <c r="Y194" s="4"/>
     </row>
-    <row r="195" spans="1:25" ht="255">
+    <row r="195" spans="1:25" ht="234">
       <c r="A195" s="5" t="s">
         <v>1426</v>
       </c>
@@ -22977,7 +23014,7 @@
       </c>
       <c r="Y195" s="4"/>
     </row>
-    <row r="196" spans="1:25" ht="409.6">
+    <row r="196" spans="1:25" ht="390">
       <c r="A196" s="5"/>
       <c r="B196" s="3" t="s">
         <v>26</v>
@@ -23032,7 +23069,7 @@
       </c>
       <c r="Y196" s="4"/>
     </row>
-    <row r="197" spans="1:25" ht="255">
+    <row r="197" spans="1:25" ht="234">
       <c r="A197" s="5" t="s">
         <v>1438</v>
       </c>
@@ -23089,7 +23126,7 @@
       </c>
       <c r="Y197" s="4"/>
     </row>
-    <row r="198" spans="1:25" ht="409.6">
+    <row r="198" spans="1:25" ht="390">
       <c r="A198" s="5" t="s">
         <v>1444</v>
       </c>
@@ -23146,7 +23183,7 @@
       </c>
       <c r="Y198" s="4"/>
     </row>
-    <row r="199" spans="1:25" ht="272">
+    <row r="199" spans="1:25" ht="249.6">
       <c r="A199" s="5" t="s">
         <v>1451</v>
       </c>
@@ -23203,7 +23240,7 @@
       </c>
       <c r="Y199" s="4"/>
     </row>
-    <row r="200" spans="1:25" ht="187">
+    <row r="200" spans="1:25" ht="171.6">
       <c r="A200" s="5" t="s">
         <v>1457</v>
       </c>
@@ -23260,7 +23297,7 @@
       </c>
       <c r="Y200" s="4"/>
     </row>
-    <row r="201" spans="1:25" ht="187">
+    <row r="201" spans="1:25" ht="171.6">
       <c r="A201" s="5" t="s">
         <v>1464</v>
       </c>
@@ -23317,7 +23354,7 @@
       </c>
       <c r="Y201" s="4"/>
     </row>
-    <row r="202" spans="1:25" ht="187">
+    <row r="202" spans="1:25" ht="171.6">
       <c r="A202" s="5" t="s">
         <v>1471</v>
       </c>
@@ -23374,7 +23411,7 @@
       </c>
       <c r="Y202" s="4"/>
     </row>
-    <row r="203" spans="1:25" ht="255">
+    <row r="203" spans="1:25" ht="218.4">
       <c r="A203" s="5" t="s">
         <v>1478</v>
       </c>
@@ -23431,7 +23468,7 @@
       </c>
       <c r="Y203" s="4"/>
     </row>
-    <row r="204" spans="1:25" ht="204">
+    <row r="204" spans="1:25" ht="187.2">
       <c r="A204" s="5" t="s">
         <v>1487</v>
       </c>
@@ -23488,7 +23525,7 @@
       </c>
       <c r="Y204" s="4"/>
     </row>
-    <row r="205" spans="1:25" ht="187">
+    <row r="205" spans="1:25" ht="171.6">
       <c r="A205" s="5" t="s">
         <v>1494</v>
       </c>
@@ -23545,7 +23582,7 @@
       </c>
       <c r="Y205" s="4"/>
     </row>
-    <row r="206" spans="1:25" ht="323">
+    <row r="206" spans="1:25" ht="296.39999999999998">
       <c r="A206" s="8" t="s">
         <v>1500</v>
       </c>
@@ -23562,17 +23599,17 @@
         <v>1503</v>
       </c>
       <c r="F206" s="7" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="G206" s="4" t="s">
         <v>1504</v>
       </c>
       <c r="H206" s="3"/>
       <c r="I206" s="7" t="s">
+        <v>1988</v>
+      </c>
+      <c r="J206" s="7" t="s">
         <v>1989</v>
-      </c>
-      <c r="J206" s="7" t="s">
-        <v>1990</v>
       </c>
       <c r="K206" s="3"/>
       <c r="L206" s="3"/>
@@ -23602,7 +23639,7 @@
       </c>
       <c r="Y206" s="4"/>
     </row>
-    <row r="207" spans="1:25" ht="409.6">
+    <row r="207" spans="1:25" ht="409.5">
       <c r="A207" s="5" t="s">
         <v>1506</v>
       </c>
@@ -23659,7 +23696,7 @@
       </c>
       <c r="Y207" s="4"/>
     </row>
-    <row r="208" spans="1:25" ht="187">
+    <row r="208" spans="1:25" ht="171.6">
       <c r="A208" s="5" t="s">
         <v>1515</v>
       </c>
@@ -23716,7 +23753,7 @@
       </c>
       <c r="Y208" s="4"/>
     </row>
-    <row r="209" spans="1:25" ht="409.6">
+    <row r="209" spans="1:25" ht="409.5">
       <c r="A209" s="5" t="s">
         <v>1522</v>
       </c>
@@ -23773,7 +23810,7 @@
       </c>
       <c r="Y209" s="4"/>
     </row>
-    <row r="210" spans="1:25" ht="409.6">
+    <row r="210" spans="1:25" ht="409.5">
       <c r="A210" s="5" t="s">
         <v>1528</v>
       </c>
@@ -23830,7 +23867,7 @@
       </c>
       <c r="Y210" s="4"/>
     </row>
-    <row r="211" spans="1:25" ht="272">
+    <row r="211" spans="1:25" ht="249.6">
       <c r="A211" s="5" t="s">
         <v>1534</v>
       </c>
@@ -23887,7 +23924,7 @@
       </c>
       <c r="Y211" s="4"/>
     </row>
-    <row r="212" spans="1:25" ht="204">
+    <row r="212" spans="1:25" ht="171.6">
       <c r="A212" s="5" t="s">
         <v>1543</v>
       </c>
@@ -23944,7 +23981,7 @@
       </c>
       <c r="Y212" s="4"/>
     </row>
-    <row r="213" spans="1:25" ht="187">
+    <row r="213" spans="1:25" ht="156">
       <c r="A213" s="5" t="s">
         <v>1552</v>
       </c>
@@ -24001,7 +24038,7 @@
       </c>
       <c r="Y213" s="4"/>
     </row>
-    <row r="214" spans="1:25" ht="409.6">
+    <row r="214" spans="1:25" ht="409.5">
       <c r="A214" s="5" t="s">
         <v>1561</v>
       </c>
@@ -24058,7 +24095,7 @@
       </c>
       <c r="Y214"/>
     </row>
-    <row r="215" spans="1:25" ht="306">
+    <row r="215" spans="1:25" ht="265.2">
       <c r="A215" s="5" t="s">
         <v>1570</v>
       </c>
@@ -24115,7 +24152,7 @@
       </c>
       <c r="Y215" s="4"/>
     </row>
-    <row r="216" spans="1:25" ht="204">
+    <row r="216" spans="1:25" ht="187.2">
       <c r="A216" s="5" t="s">
         <v>1577</v>
       </c>
@@ -24172,7 +24209,7 @@
       </c>
       <c r="Y216" s="4"/>
     </row>
-    <row r="217" spans="1:25" ht="187">
+    <row r="217" spans="1:25" ht="156">
       <c r="A217" s="5" t="s">
         <v>1584</v>
       </c>
@@ -24229,7 +24266,7 @@
       </c>
       <c r="Y217"/>
     </row>
-    <row r="218" spans="1:25" ht="187">
+    <row r="218" spans="1:25" ht="171.6">
       <c r="A218" s="5" t="s">
         <v>1593</v>
       </c>
@@ -24286,7 +24323,7 @@
       </c>
       <c r="Y218" s="4"/>
     </row>
-    <row r="219" spans="1:25" ht="409.6">
+    <row r="219" spans="1:25" ht="390">
       <c r="A219" s="5" t="s">
         <v>1600</v>
       </c>
@@ -24343,9 +24380,9 @@
       </c>
       <c r="Y219" s="4"/>
     </row>
-    <row r="220" spans="1:25" ht="255">
+    <row r="220" spans="1:25" ht="218.4">
       <c r="A220" s="13" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>48</v>
@@ -24400,7 +24437,7 @@
       </c>
       <c r="Y220"/>
     </row>
-    <row r="221" spans="1:25" ht="289">
+    <row r="221" spans="1:25" ht="265.2">
       <c r="A221" s="5" t="s">
         <v>1612</v>
       </c>
@@ -24457,7 +24494,7 @@
       </c>
       <c r="Y221" s="4"/>
     </row>
-    <row r="222" spans="1:25" ht="187">
+    <row r="222" spans="1:25" ht="171.6">
       <c r="A222" s="5" t="s">
         <v>1619</v>
       </c>
@@ -24514,7 +24551,7 @@
       </c>
       <c r="Y222" s="4"/>
     </row>
-    <row r="223" spans="1:25" ht="187">
+    <row r="223" spans="1:25" ht="171.6">
       <c r="A223" s="5" t="s">
         <v>1626</v>
       </c>
@@ -24571,7 +24608,7 @@
       </c>
       <c r="Y223" s="4"/>
     </row>
-    <row r="224" spans="1:25" ht="289">
+    <row r="224" spans="1:25" ht="265.2">
       <c r="A224" s="5" t="s">
         <v>1632</v>
       </c>
@@ -24628,7 +24665,7 @@
       </c>
       <c r="Y224" s="4"/>
     </row>
-    <row r="225" spans="1:25" ht="289">
+    <row r="225" spans="1:25" ht="249.6">
       <c r="A225" s="5" t="s">
         <v>1639</v>
       </c>
@@ -24685,7 +24722,7 @@
       </c>
       <c r="Y225" s="16"/>
     </row>
-    <row r="226" spans="1:25" ht="289">
+    <row r="226" spans="1:25" ht="265.2">
       <c r="A226" s="5" t="s">
         <v>1647</v>
       </c>
@@ -24742,7 +24779,7 @@
       </c>
       <c r="Y226" s="4"/>
     </row>
-    <row r="227" spans="1:25" ht="238">
+    <row r="227" spans="1:25" ht="218.4">
       <c r="A227" s="5" t="s">
         <v>1654</v>
       </c>
@@ -24799,7 +24836,7 @@
       </c>
       <c r="Y227" s="4"/>
     </row>
-    <row r="228" spans="1:25" ht="388">
+    <row r="228" spans="1:25" ht="343.2">
       <c r="A228" s="8" t="s">
         <v>1663</v>
       </c>
@@ -24852,11 +24889,11 @@
         <v>2367</v>
       </c>
       <c r="X228" s="7" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="Y228" s="4"/>
     </row>
-    <row r="229" spans="1:25" ht="409.6">
+    <row r="229" spans="1:25" ht="409.5">
       <c r="A229" s="5" t="s">
         <v>1670</v>
       </c>
@@ -24913,7 +24950,7 @@
       </c>
       <c r="Y229" s="4"/>
     </row>
-    <row r="230" spans="1:25" ht="238">
+    <row r="230" spans="1:25" ht="218.4">
       <c r="A230" s="5" t="s">
         <v>1679</v>
       </c>
@@ -24970,7 +25007,7 @@
       </c>
       <c r="Y230" s="4"/>
     </row>
-    <row r="231" spans="1:25" ht="272">
+    <row r="231" spans="1:25" ht="249.6">
       <c r="A231" s="5" t="s">
         <v>1688</v>
       </c>
@@ -25027,7 +25064,7 @@
       </c>
       <c r="Y231" s="4"/>
     </row>
-    <row r="232" spans="1:25" ht="272">
+    <row r="232" spans="1:25" ht="234">
       <c r="A232" s="8" t="s">
         <v>1697</v>
       </c>
@@ -25051,10 +25088,10 @@
       </c>
       <c r="H232" s="3"/>
       <c r="I232" s="7" t="s">
+        <v>1959</v>
+      </c>
+      <c r="J232" s="7" t="s">
         <v>1960</v>
-      </c>
-      <c r="J232" s="7" t="s">
-        <v>1961</v>
       </c>
       <c r="K232" s="3"/>
       <c r="L232" s="3"/>
@@ -25084,7 +25121,7 @@
       </c>
       <c r="Y232" s="4"/>
     </row>
-    <row r="233" spans="1:25" ht="306">
+    <row r="233" spans="1:25" ht="265.2">
       <c r="A233" s="5" t="s">
         <v>1704</v>
       </c>
@@ -25141,7 +25178,7 @@
       </c>
       <c r="Y233" s="4"/>
     </row>
-    <row r="234" spans="1:25" ht="153">
+    <row r="234" spans="1:25" ht="140.4">
       <c r="A234" s="5" t="s">
         <v>1712</v>
       </c>
@@ -25198,7 +25235,7 @@
       </c>
       <c r="Y234" s="4"/>
     </row>
-    <row r="235" spans="1:25" ht="272">
+    <row r="235" spans="1:25" ht="249.6">
       <c r="A235" s="5" t="s">
         <v>1721</v>
       </c>
@@ -25255,7 +25292,7 @@
       </c>
       <c r="Y235" s="4"/>
     </row>
-    <row r="236" spans="1:25" ht="409.6">
+    <row r="236" spans="1:25" ht="409.5">
       <c r="A236" s="8" t="s">
         <v>1729</v>
       </c>
@@ -25272,17 +25309,17 @@
         <v>1731</v>
       </c>
       <c r="F236" s="7" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="G236" s="4" t="s">
         <v>1054</v>
       </c>
       <c r="H236" s="3"/>
       <c r="I236" s="7" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="J236" s="7" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="K236" s="3"/>
       <c r="L236" s="3"/>
@@ -25312,7 +25349,7 @@
       </c>
       <c r="Y236" s="4"/>
     </row>
-    <row r="237" spans="1:25" ht="272">
+    <row r="237" spans="1:25" ht="234">
       <c r="A237" s="8" t="s">
         <v>1732</v>
       </c>
@@ -25329,14 +25366,14 @@
         <v>1735</v>
       </c>
       <c r="F237" s="7" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="G237" s="4" t="s">
         <v>1736</v>
       </c>
       <c r="H237" s="3"/>
       <c r="I237" s="7" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="J237" s="4" t="s">
         <v>1737</v>
@@ -25369,7 +25406,7 @@
       </c>
       <c r="Y237" s="4"/>
     </row>
-    <row r="238" spans="1:25" ht="255">
+    <row r="238" spans="1:25" ht="234">
       <c r="A238" s="5" t="s">
         <v>1739</v>
       </c>
@@ -25426,7 +25463,7 @@
       </c>
       <c r="Y238" s="4"/>
     </row>
-    <row r="239" spans="1:25" ht="409.6">
+    <row r="239" spans="1:25" ht="405.6">
       <c r="A239" s="8" t="s">
         <v>1746</v>
       </c>
@@ -25443,17 +25480,17 @@
         <v>1749</v>
       </c>
       <c r="F239" s="7" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="G239" s="4" t="s">
         <v>1750</v>
       </c>
       <c r="H239" s="3"/>
       <c r="I239" s="7" t="s">
+        <v>1966</v>
+      </c>
+      <c r="J239" s="7" t="s">
         <v>1967</v>
-      </c>
-      <c r="J239" s="7" t="s">
-        <v>1968</v>
       </c>
       <c r="K239" s="3"/>
       <c r="L239" s="3"/>
@@ -25483,12 +25520,12 @@
       </c>
       <c r="Y239" s="4"/>
     </row>
-    <row r="240" spans="1:25" ht="255">
+    <row r="240" spans="1:25" ht="234">
       <c r="A240" s="8" t="s">
         <v>1752</v>
       </c>
       <c r="B240" s="11" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="C240" s="3" t="s">
         <v>27</v>
@@ -25539,10 +25576,10 @@
         <v>37</v>
       </c>
       <c r="Y240" s="12" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
     </row>
-    <row r="241" spans="1:25" ht="409.6">
+    <row r="241" spans="1:25" ht="405.6">
       <c r="A241" s="8" t="s">
         <v>1759</v>
       </c>
@@ -25566,10 +25603,10 @@
       </c>
       <c r="H241" s="3"/>
       <c r="I241" s="7" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="J241" s="7" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="K241" s="3"/>
       <c r="L241" s="3"/>
@@ -25599,7 +25636,7 @@
       </c>
       <c r="Y241" s="4"/>
     </row>
-    <row r="242" spans="1:25" ht="221">
+    <row r="242" spans="1:25" ht="187.2">
       <c r="A242" s="5" t="s">
         <v>1765</v>
       </c>
@@ -25656,7 +25693,7 @@
       </c>
       <c r="Y242" s="16"/>
     </row>
-    <row r="243" spans="1:25" ht="323">
+    <row r="243" spans="1:25" ht="280.8">
       <c r="A243" s="5" t="s">
         <v>1772</v>
       </c>
@@ -25713,7 +25750,7 @@
       </c>
       <c r="Y243" s="16"/>
     </row>
-    <row r="244" spans="1:25" ht="340">
+    <row r="244" spans="1:25" ht="312">
       <c r="A244" s="5" t="s">
         <v>1778</v>
       </c>
@@ -25770,7 +25807,7 @@
       </c>
       <c r="Y244" s="4"/>
     </row>
-    <row r="245" spans="1:25" ht="323">
+    <row r="245" spans="1:25" ht="249.6">
       <c r="A245" s="5" t="s">
         <v>1785</v>
       </c>
@@ -25827,7 +25864,7 @@
       </c>
       <c r="Y245" s="16"/>
     </row>
-    <row r="246" spans="1:25" ht="187">
+    <row r="246" spans="1:25" ht="171.6">
       <c r="A246" s="5" t="s">
         <v>1789</v>
       </c>
@@ -25884,7 +25921,7 @@
       </c>
       <c r="Y246" s="4"/>
     </row>
-    <row r="247" spans="1:25" ht="221">
+    <row r="247" spans="1:25" ht="202.8">
       <c r="A247" s="5" t="s">
         <v>1796</v>
       </c>
@@ -25941,7 +25978,7 @@
       </c>
       <c r="Y247" s="16"/>
     </row>
-    <row r="248" spans="1:25" ht="340">
+    <row r="248" spans="1:25" ht="312">
       <c r="A248" s="5" t="s">
         <v>1800</v>
       </c>
@@ -25998,7 +26035,7 @@
       </c>
       <c r="Y248" s="4"/>
     </row>
-    <row r="249" spans="1:25" ht="409.6">
+    <row r="249" spans="1:25" ht="409.5">
       <c r="A249" s="5" t="s">
         <v>1807</v>
       </c>
@@ -26055,7 +26092,7 @@
       </c>
       <c r="Y249" s="4"/>
     </row>
-    <row r="250" spans="1:25" ht="255">
+    <row r="250" spans="1:25" ht="234">
       <c r="A250" s="5" t="s">
         <v>1814</v>
       </c>
@@ -26112,7 +26149,7 @@
       </c>
       <c r="Y250" s="4"/>
     </row>
-    <row r="251" spans="1:25" ht="187">
+    <row r="251" spans="1:25" ht="171.6">
       <c r="A251" s="5" t="s">
         <v>1821</v>
       </c>
@@ -26169,7 +26206,7 @@
       </c>
       <c r="Y251" s="4"/>
     </row>
-    <row r="252" spans="1:25" ht="187">
+    <row r="252" spans="1:25" ht="171.6">
       <c r="A252" s="5" t="s">
         <v>1828</v>
       </c>
@@ -26226,7 +26263,7 @@
       </c>
       <c r="Y252" s="4"/>
     </row>
-    <row r="253" spans="1:25" ht="221">
+    <row r="253" spans="1:25" ht="202.8">
       <c r="A253" s="5" t="s">
         <v>1835</v>
       </c>
@@ -26283,7 +26320,7 @@
       </c>
       <c r="Y253" s="4"/>
     </row>
-    <row r="254" spans="1:25" ht="187">
+    <row r="254" spans="1:25" ht="171.6">
       <c r="A254" s="5" t="s">
         <v>1842</v>
       </c>
@@ -26340,7 +26377,7 @@
       </c>
       <c r="Y254" s="4"/>
     </row>
-    <row r="255" spans="1:25" ht="409.6">
+    <row r="255" spans="1:25" ht="390">
       <c r="A255" s="5" t="s">
         <v>1849</v>
       </c>
@@ -26397,7 +26434,7 @@
       </c>
       <c r="Y255" s="16"/>
     </row>
-    <row r="256" spans="1:25" ht="187">
+    <row r="256" spans="1:25" ht="171.6">
       <c r="A256" s="5" t="s">
         <v>1856</v>
       </c>
@@ -26454,7 +26491,7 @@
       </c>
       <c r="Y256" s="4"/>
     </row>
-    <row r="257" spans="1:25" ht="340">
+    <row r="257" spans="1:25" ht="312">
       <c r="A257" s="5" t="s">
         <v>1863</v>
       </c>
@@ -26511,7 +26548,7 @@
       </c>
       <c r="Y257" s="4"/>
     </row>
-    <row r="258" spans="1:25" ht="221">
+    <row r="258" spans="1:25" ht="202.8">
       <c r="A258" s="5" t="s">
         <v>1870</v>
       </c>
@@ -26568,8 +26605,8 @@
       </c>
       <c r="Y258" s="4"/>
     </row>
-    <row r="259" spans="1:25" ht="306">
-      <c r="A259" s="5" t="s">
+    <row r="259" spans="1:25" ht="280.8">
+      <c r="A259" s="8" t="s">
         <v>1877</v>
       </c>
       <c r="B259" s="3" t="s">
@@ -26620,39 +26657,41 @@
       <c r="W259" s="3">
         <v>2367</v>
       </c>
-      <c r="X259" s="4" t="s">
+      <c r="X259" s="17" t="s">
+        <v>1993</v>
+      </c>
+      <c r="Y259" s="17" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="260" spans="1:25" ht="409.5">
+      <c r="A260" s="5" t="s">
         <v>1885</v>
-      </c>
-      <c r="Y259" s="4"/>
-    </row>
-    <row r="260" spans="1:25" ht="409.6">
-      <c r="A260" s="5" t="s">
-        <v>1886</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C260" s="3" t="s">
+        <v>1886</v>
+      </c>
+      <c r="D260" s="3" t="s">
         <v>1887</v>
       </c>
-      <c r="D260" s="3" t="s">
+      <c r="E260" s="3" t="s">
+        <v>1886</v>
+      </c>
+      <c r="F260" s="4" t="s">
         <v>1888</v>
       </c>
-      <c r="E260" s="3" t="s">
-        <v>1887</v>
-      </c>
-      <c r="F260" s="4" t="s">
+      <c r="G260" s="4" t="s">
         <v>1889</v>
-      </c>
-      <c r="G260" s="4" t="s">
-        <v>1890</v>
       </c>
       <c r="H260" s="3"/>
       <c r="I260" s="4" t="s">
+        <v>1890</v>
+      </c>
+      <c r="J260" s="4" t="s">
         <v>1891</v>
-      </c>
-      <c r="J260" s="4" t="s">
-        <v>1892</v>
       </c>
       <c r="K260" s="3"/>
       <c r="L260" s="3"/>
@@ -26678,13 +26717,13 @@
         <v>2367</v>
       </c>
       <c r="X260" s="4" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="Y260" s="4"/>
     </row>
-    <row r="261" spans="1:25" ht="289">
+    <row r="261" spans="1:25" ht="249.6">
       <c r="A261" s="5" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="B261" s="3" t="s">
         <v>26</v>
@@ -26693,23 +26732,23 @@
         <v>39</v>
       </c>
       <c r="D261" s="3" t="s">
+        <v>1894</v>
+      </c>
+      <c r="E261" s="3" t="s">
         <v>1895</v>
       </c>
-      <c r="E261" s="3" t="s">
+      <c r="F261" s="4" t="s">
         <v>1896</v>
-      </c>
-      <c r="F261" s="4" t="s">
-        <v>1897</v>
       </c>
       <c r="G261" s="4" t="s">
         <v>598</v>
       </c>
       <c r="H261" s="3"/>
       <c r="I261" s="4" t="s">
+        <v>1897</v>
+      </c>
+      <c r="J261" s="4" t="s">
         <v>1898</v>
-      </c>
-      <c r="J261" s="4" t="s">
-        <v>1899</v>
       </c>
       <c r="K261" s="3"/>
       <c r="L261" s="3"/>
@@ -26739,34 +26778,34 @@
       </c>
       <c r="Y261" s="4"/>
     </row>
-    <row r="262" spans="1:25" ht="388">
+    <row r="262" spans="1:25" ht="343.2">
       <c r="A262" s="5" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B262" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C262" s="3" t="s">
+        <v>1900</v>
+      </c>
+      <c r="D262" s="3" t="s">
         <v>1901</v>
       </c>
-      <c r="D262" s="3" t="s">
+      <c r="E262" s="3" t="s">
         <v>1902</v>
       </c>
-      <c r="E262" s="3" t="s">
+      <c r="F262" s="4" t="s">
         <v>1903</v>
       </c>
-      <c r="F262" s="4" t="s">
+      <c r="G262" s="4" t="s">
         <v>1904</v>
-      </c>
-      <c r="G262" s="4" t="s">
-        <v>1905</v>
       </c>
       <c r="H262" s="3"/>
       <c r="I262" s="4" t="s">
+        <v>1905</v>
+      </c>
+      <c r="J262" s="4" t="s">
         <v>1906</v>
-      </c>
-      <c r="J262" s="4" t="s">
-        <v>1907</v>
       </c>
       <c r="K262" s="3"/>
       <c r="L262" s="3"/>
@@ -26792,38 +26831,38 @@
         <v>2367</v>
       </c>
       <c r="X262" s="4" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="Y262" s="4"/>
     </row>
-    <row r="263" spans="1:25" ht="372">
+    <row r="263" spans="1:25" ht="343.2">
       <c r="A263" s="5" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B263" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C263" s="3" t="s">
+        <v>1909</v>
+      </c>
+      <c r="D263" s="3" t="s">
         <v>1910</v>
       </c>
-      <c r="D263" s="3" t="s">
+      <c r="E263" s="3" t="s">
         <v>1911</v>
       </c>
-      <c r="E263" s="3" t="s">
+      <c r="F263" s="4" t="s">
         <v>1912</v>
       </c>
-      <c r="F263" s="4" t="s">
+      <c r="G263" s="4" t="s">
         <v>1913</v>
-      </c>
-      <c r="G263" s="4" t="s">
-        <v>1914</v>
       </c>
       <c r="H263" s="3"/>
       <c r="I263" s="4" t="s">
+        <v>1914</v>
+      </c>
+      <c r="J263" s="4" t="s">
         <v>1915</v>
-      </c>
-      <c r="J263" s="4" t="s">
-        <v>1916</v>
       </c>
       <c r="K263" s="3"/>
       <c r="L263" s="3"/>
@@ -26849,38 +26888,38 @@
         <v>2367</v>
       </c>
       <c r="X263" s="4" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="Y263" s="4"/>
     </row>
-    <row r="264" spans="1:25" ht="356">
+    <row r="264" spans="1:25" ht="327.60000000000002">
       <c r="A264" s="5" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B264" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="D264" s="3" t="s">
+        <v>1918</v>
+      </c>
+      <c r="E264" s="3" t="s">
         <v>1919</v>
       </c>
-      <c r="E264" s="3" t="s">
+      <c r="F264" s="4" t="s">
         <v>1920</v>
       </c>
-      <c r="F264" s="4" t="s">
+      <c r="G264" s="4" t="s">
         <v>1921</v>
-      </c>
-      <c r="G264" s="4" t="s">
-        <v>1922</v>
       </c>
       <c r="H264" s="3"/>
       <c r="I264" s="4" t="s">
+        <v>1922</v>
+      </c>
+      <c r="J264" s="4" t="s">
         <v>1923</v>
-      </c>
-      <c r="J264" s="4" t="s">
-        <v>1924</v>
       </c>
       <c r="K264" s="3"/>
       <c r="L264" s="3"/>
@@ -26906,38 +26945,38 @@
         <v>2367</v>
       </c>
       <c r="X264" s="4" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="Y264" s="4"/>
     </row>
-    <row r="265" spans="1:25" ht="372">
+    <row r="265" spans="1:25" ht="343.2">
       <c r="A265" s="5" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B265" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="D265" s="3" t="s">
+        <v>1925</v>
+      </c>
+      <c r="E265" s="3" t="s">
         <v>1926</v>
       </c>
-      <c r="E265" s="3" t="s">
+      <c r="F265" s="4" t="s">
         <v>1927</v>
       </c>
-      <c r="F265" s="4" t="s">
+      <c r="G265" s="4" t="s">
         <v>1928</v>
-      </c>
-      <c r="G265" s="4" t="s">
-        <v>1929</v>
       </c>
       <c r="H265" s="3"/>
       <c r="I265" s="4" t="s">
+        <v>1929</v>
+      </c>
+      <c r="J265" s="4" t="s">
         <v>1930</v>
-      </c>
-      <c r="J265" s="4" t="s">
-        <v>1931</v>
       </c>
       <c r="K265" s="3"/>
       <c r="L265" s="3"/>
@@ -26963,7 +27002,7 @@
         <v>2367</v>
       </c>
       <c r="X265" s="4" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="Y265" s="4"/>
     </row>

</xml_diff>

<commit_message>
Updated to deprecate tests related to CM-5(6)
(CM-5(6) is not cited in CMS ARS 3.1)
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-red-hat-enterprise-linux-6-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-red-hat-enterprise-linux-6-stig-overlay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\CMS_InSpec_Profile_to_NISTSecurityControl_Maps_06132019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D92EAA14-5F34-4BAF-969A-86AFAE6FC28B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EEABF819-0A0A-4AB9-90CF-7EF769D39E75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-552" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-rhel6-stig" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3460" uniqueCount="1995">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3464" uniqueCount="1995">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -11446,7 +11446,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -11493,6 +11493,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -13321,11 +13336,11 @@
       <c r="Y25"/>
     </row>
     <row r="26" spans="1:25" ht="358.8">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>48</v>
+      <c r="B26" s="18" t="s">
+        <v>1980</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>210</v>
@@ -13375,14 +13390,16 @@
       <c r="X26" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="Y26" s="4"/>
+      <c r="Y26" s="21" t="s">
+        <v>1979</v>
+      </c>
     </row>
     <row r="27" spans="1:25" ht="409.5">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>48</v>
+      <c r="B27" s="18" t="s">
+        <v>1980</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>210</v>
@@ -13432,7 +13449,9 @@
       <c r="X27" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="Y27" s="4"/>
+      <c r="Y27" s="22" t="s">
+        <v>1979</v>
+      </c>
     </row>
     <row r="28" spans="1:25" ht="140.4">
       <c r="A28" s="5" t="s">
@@ -13549,11 +13568,11 @@
       <c r="Y29"/>
     </row>
     <row r="30" spans="1:25" ht="312">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>48</v>
+      <c r="B30" s="18" t="s">
+        <v>1980</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>210</v>
@@ -13603,7 +13622,9 @@
       <c r="X30" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="Y30" s="4"/>
+      <c r="Y30" s="19" t="s">
+        <v>1979</v>
+      </c>
     </row>
     <row r="31" spans="1:25" ht="409.5">
       <c r="A31" s="5" t="s">
@@ -13720,11 +13741,11 @@
       <c r="Y32" s="4"/>
     </row>
     <row r="33" spans="1:25" ht="327.60000000000002">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>48</v>
+      <c r="B33" s="18" t="s">
+        <v>1980</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>210</v>
@@ -13774,7 +13795,9 @@
       <c r="X33" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="Y33" s="4"/>
+      <c r="Y33" s="20" t="s">
+        <v>1979</v>
+      </c>
     </row>
     <row r="34" spans="1:25" ht="171.6">
       <c r="A34" s="5" t="s">

</xml_diff>